<commit_message>
split read_tdf.py out for readability
</commit_message>
<xml_diff>
--- a/Subject Allocations.xlsx
+++ b/Subject Allocations.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Whole Staff" sheetId="1" r:id="rId1"/>
+    <sheet name="All Staff" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="484">
   <si>
     <t>2022 Teaching Staff Sem 2</t>
   </si>
   <si>
-    <t>30/06/2022 12:36:17</t>
+    <t>30/06/2022 13:49:51</t>
   </si>
   <si>
     <t>M - 6 4 3 PD 5</t>
@@ -181,6 +181,9 @@
     <t>English</t>
   </si>
   <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
     <t>Mel</t>
   </si>
   <si>
@@ -313,6 +316,9 @@
     <t>M2</t>
   </si>
   <si>
+    <t>SC4</t>
+  </si>
+  <si>
     <t>Art</t>
   </si>
   <si>
@@ -355,7 +361,7 @@
     <t>M7</t>
   </si>
   <si>
-    <t>Mathematics</t>
+    <t>SC2</t>
   </si>
   <si>
     <t>SU3</t>
@@ -511,12 +517,6 @@
     <t>M4</t>
   </si>
   <si>
-    <t>SC2</t>
-  </si>
-  <si>
-    <t>SC4</t>
-  </si>
-  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -1120,6 +1120,9 @@
     <t>Art (Music)</t>
   </si>
   <si>
+    <t>Language and Culture</t>
+  </si>
+  <si>
     <t>Sarah</t>
   </si>
   <si>
@@ -1279,6 +1282,9 @@
     <t>SANM</t>
   </si>
   <si>
+    <t>Food Technology</t>
+  </si>
+  <si>
     <t>Roopali</t>
   </si>
   <si>
@@ -1376,6 +1382,9 @@
   </si>
   <si>
     <t>M9</t>
+  </si>
+  <si>
+    <t>Cross Disc</t>
   </si>
   <si>
     <t>SWDRP</t>
@@ -2183,13 +2192,10 @@
         <v>51</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="14" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2209,13 +2215,10 @@
         <v>52</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="14" t="s">
         <v>54</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2237,27 +2240,24 @@
       <c r="G18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="J18" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>38</v>
@@ -2266,12 +2266,12 @@
         <v>54</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>8</v>
@@ -2280,17 +2280,17 @@
         <v>21</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>22</v>
@@ -2298,21 +2298,21 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>33</v>
@@ -2323,47 +2323,47 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>41</v>
@@ -2372,7 +2372,7 @@
         <v>22</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H32" s="14" t="s">
         <v>22</v>
@@ -2383,53 +2383,53 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>20</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>38</v>
@@ -2458,7 +2458,7 @@
         <v>25</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>25</v>
@@ -2466,27 +2466,27 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>33</v>
@@ -2495,29 +2495,29 @@
         <v>20</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>8</v>
@@ -2529,35 +2529,35 @@
         <v>24</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H44" s="14" t="s">
         <v>48</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>38</v>
@@ -2569,47 +2569,47 @@
         <v>49</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I45" s="14" t="s">
         <v>50</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>41</v>
@@ -2618,7 +2618,7 @@
         <v>41</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>22</v>
@@ -2629,133 +2629,133 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J52" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D53" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="H53" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>49</v>
       </c>
       <c r="J53" s="14" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>20</v>
@@ -2763,18 +2763,18 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>41</v>
@@ -2788,16 +2788,16 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H61" s="14" t="s">
         <v>23</v>
@@ -2808,108 +2808,108 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H66" s="14" t="s">
         <v>47</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G68" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H68" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B69" s="14" t="s">
         <v>38</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>22</v>
@@ -2918,58 +2918,58 @@
         <v>22</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G73" s="14" t="s">
         <v>39</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D76" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>33</v>
@@ -2978,7 +2978,7 @@
         <v>33</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J76" s="14" t="s">
         <v>41</v>
@@ -2986,168 +2986,150 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J77" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J78" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>161</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="I84" s="14" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
       <c r="J84" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="E85" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G85" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="H85" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="I85" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="J85" s="14" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G86" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="I86" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J86" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3155,7 +3137,7 @@
         <v>168</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E88" s="14" t="s">
         <v>20</v>
@@ -3224,7 +3206,7 @@
         <v>22</v>
       </c>
       <c r="J92" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3247,7 +3229,7 @@
         <v>183</v>
       </c>
       <c r="J93" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3324,7 +3306,7 @@
         <v>8</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F98" s="14" t="s">
         <v>171</v>
@@ -3333,10 +3315,10 @@
         <v>188</v>
       </c>
       <c r="I98" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J98" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -3353,13 +3335,13 @@
         <v>20</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H100" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I100" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -3376,7 +3358,7 @@
         <v>173</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G101" s="14" t="s">
         <v>194</v>
@@ -3422,22 +3404,19 @@
         <v>53</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="F104" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G104" s="14" t="s">
-        <v>97</v>
-      </c>
       <c r="H104" s="14" t="s">
         <v>53</v>
       </c>
       <c r="I104" s="14" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="J104" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -3451,14 +3430,11 @@
         <v>49</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="F105" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G105" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="H105" s="14" t="s">
         <v>199</v>
       </c>
@@ -3466,7 +3442,7 @@
         <v>50</v>
       </c>
       <c r="J105" s="14" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -3477,25 +3453,22 @@
         <v>8</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J106" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -3526,13 +3499,13 @@
         <v>20</v>
       </c>
       <c r="E109" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I109" s="14" t="s">
         <v>204</v>
@@ -3575,7 +3548,7 @@
         <v>33</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -3586,10 +3559,10 @@
         <v>38</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G113" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H113" s="14" t="s">
         <v>209</v>
@@ -3603,7 +3576,7 @@
         <v>8</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G114" s="14" t="s">
         <v>27</v>
@@ -3677,7 +3650,7 @@
         <v>20</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G120" s="14" t="s">
         <v>20</v>
@@ -3809,13 +3782,13 @@
         <v>33</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H128" s="14" t="s">
         <v>41</v>
       </c>
       <c r="J128" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -3868,7 +3841,7 @@
         <v>244</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -3884,16 +3857,16 @@
         <v>247</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F136" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G136" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J136" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="G136" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J136" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -3901,7 +3874,7 @@
         <v>248</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E137" s="14" t="s">
         <v>250</v>
@@ -3921,10 +3894,10 @@
         <v>249</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F138" s="14" t="s">
         <v>42</v>
@@ -3933,7 +3906,7 @@
         <v>253</v>
       </c>
       <c r="J138" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -3944,7 +3917,7 @@
         <v>20</v>
       </c>
       <c r="F140" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G140" s="14" t="s">
         <v>33</v>
@@ -3958,13 +3931,13 @@
         <v>41</v>
       </c>
       <c r="E141" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F141" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G141" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -3972,7 +3945,7 @@
         <v>257</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E142" s="14" t="s">
         <v>203</v>
@@ -3998,7 +3971,7 @@
         <v>41</v>
       </c>
       <c r="I144" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J144" s="14" t="s">
         <v>33</v>
@@ -4061,7 +4034,7 @@
         <v>22</v>
       </c>
       <c r="G148" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I148" s="14" t="s">
         <v>22</v>
@@ -4081,16 +4054,16 @@
         <v>26</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G149" s="14" t="s">
         <v>269</v>
       </c>
       <c r="I149" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J149" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -4121,7 +4094,7 @@
         <v>271</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E152" s="14" t="s">
         <v>33</v>
@@ -4130,7 +4103,7 @@
         <v>33</v>
       </c>
       <c r="G152" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I152" s="14" t="s">
         <v>22</v>
@@ -4205,7 +4178,7 @@
         <v>22</v>
       </c>
       <c r="H156" s="14" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -4225,7 +4198,7 @@
         <v>233</v>
       </c>
       <c r="H157" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -4245,7 +4218,7 @@
         <v>234</v>
       </c>
       <c r="H158" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -4259,10 +4232,10 @@
         <v>41</v>
       </c>
       <c r="H160" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I160" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J160" s="14" t="s">
         <v>41</v>
@@ -4325,7 +4298,7 @@
         <v>20</v>
       </c>
       <c r="G164" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H164" s="14" t="s">
         <v>33</v>
@@ -4342,10 +4315,10 @@
         <v>33</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E165" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G165" s="14" t="s">
         <v>295</v>
@@ -4385,7 +4358,7 @@
         <v>297</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F168" s="14" t="s">
         <v>41</v>
@@ -4437,22 +4410,22 @@
         <v>8</v>
       </c>
       <c r="D170" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F170" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="F170" s="14" t="s">
-        <v>136</v>
       </c>
       <c r="G170" s="14" t="s">
         <v>303</v>
       </c>
       <c r="H170" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I170" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J170" s="14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="172" spans="1:10">
@@ -4460,10 +4433,10 @@
         <v>305</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="173" spans="1:10">
@@ -4471,7 +4444,7 @@
         <v>306</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E173" s="14" t="s">
         <v>309</v>
@@ -4516,7 +4489,7 @@
         <v>313</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E177" s="14" t="s">
         <v>187</v>
@@ -4638,7 +4611,7 @@
         <v>325</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D186" s="14" t="s">
         <v>238</v>
@@ -4689,10 +4662,10 @@
         <v>308</v>
       </c>
       <c r="G190" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H190" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="192" spans="1:10">
@@ -4774,7 +4747,7 @@
         <v>336</v>
       </c>
       <c r="J197" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="198" spans="1:10">
@@ -4828,7 +4801,7 @@
         <v>22</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E201" s="14" t="s">
         <v>276</v>
@@ -4871,13 +4844,13 @@
         <v>343</v>
       </c>
       <c r="G204" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I204" s="14" t="s">
         <v>22</v>
       </c>
       <c r="J204" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="205" spans="1:10">
@@ -4885,7 +4858,7 @@
         <v>344</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G205" s="14" t="s">
         <v>346</v>
@@ -4919,10 +4892,7 @@
         <v>349</v>
       </c>
       <c r="E208" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J208" s="14" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="209" spans="1:10">
@@ -4930,13 +4900,10 @@
         <v>350</v>
       </c>
       <c r="B209" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E209" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="J209" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="210" spans="1:10">
@@ -4947,10 +4914,7 @@
         <v>352</v>
       </c>
       <c r="E210" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J210" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="212" spans="1:10">
@@ -4958,7 +4922,7 @@
         <v>353</v>
       </c>
       <c r="G212" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="213" spans="1:10">
@@ -4977,7 +4941,7 @@
         <v>355</v>
       </c>
       <c r="B214" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G214" s="14" t="s">
         <v>348</v>
@@ -4985,7 +4949,7 @@
     </row>
     <row r="216" spans="1:10">
       <c r="A216" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D216" s="14" t="s">
         <v>41</v>
@@ -5005,13 +4969,13 @@
         <v>38</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E217" s="14" t="s">
         <v>315</v>
       </c>
       <c r="J217" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="218" spans="1:10">
@@ -5065,10 +5029,10 @@
         <v>290</v>
       </c>
       <c r="E221" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F221" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G221" s="14" t="s">
         <v>189</v>
@@ -5088,22 +5052,22 @@
         <v>8</v>
       </c>
       <c r="D222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J222" s="14" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="224" spans="1:10">
@@ -5111,22 +5075,19 @@
         <v>363</v>
       </c>
       <c r="D224" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E224" s="14" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="G224" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H224" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I224" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="J224" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="225" spans="1:10">
@@ -5137,10 +5098,10 @@
         <v>41</v>
       </c>
       <c r="D225" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E225" s="14" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="G225" s="14" t="s">
         <v>54</v>
@@ -5149,10 +5110,7 @@
         <v>367</v>
       </c>
       <c r="I225" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J225" s="14" t="s">
-        <v>54</v>
+        <v>368</v>
       </c>
     </row>
     <row r="226" spans="1:10">
@@ -5177,13 +5135,10 @@
       <c r="I226" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="J226" s="14" t="s">
-        <v>366</v>
-      </c>
     </row>
     <row r="228" spans="1:10">
       <c r="A228" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D228" s="14" t="s">
         <v>33</v>
@@ -5203,13 +5158,13 @@
     </row>
     <row r="229" spans="1:10">
       <c r="A229" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B229" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D229" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E229" s="14" t="s">
         <v>230</v>
@@ -5226,7 +5181,7 @@
     </row>
     <row r="230" spans="1:10">
       <c r="A230" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B230" s="14" t="s">
         <v>8</v>
@@ -5235,13 +5190,13 @@
         <v>231</v>
       </c>
       <c r="E230" s="14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H230" s="14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I230" s="14" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="J230" s="14" t="s">
         <v>231</v>
@@ -5249,13 +5204,13 @@
     </row>
     <row r="232" spans="1:10">
       <c r="A232" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D232" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E232" s="14" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F232" s="14" t="s">
         <v>22</v>
@@ -5269,13 +5224,13 @@
     </row>
     <row r="233" spans="1:10">
       <c r="A233" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B233" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D233" s="14" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F233" s="14" t="s">
         <v>189</v>
@@ -5284,12 +5239,12 @@
         <v>26</v>
       </c>
       <c r="I233" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="234" spans="1:10">
       <c r="A234" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B234" s="14" t="s">
         <v>270</v>
@@ -5312,7 +5267,7 @@
     </row>
     <row r="236" spans="1:10">
       <c r="A236" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G236" s="14" t="s">
         <v>20</v>
@@ -5320,18 +5275,18 @@
     </row>
     <row r="237" spans="1:10">
       <c r="A237" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B237" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G237" s="14" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="238" spans="1:10">
       <c r="A238" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B238" s="14" t="s">
         <v>24</v>
@@ -5342,7 +5297,7 @@
     </row>
     <row r="240" spans="1:10">
       <c r="A240" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D240" s="14" t="s">
         <v>41</v>
@@ -5351,7 +5306,7 @@
         <v>33</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G240" s="14" t="s">
         <v>33</v>
@@ -5359,19 +5314,19 @@
     </row>
     <row r="241" spans="1:10">
       <c r="A241" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B241" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E241" s="14" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F241" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G241" s="14" t="s">
         <v>204</v>
@@ -5379,27 +5334,27 @@
     </row>
     <row r="242" spans="1:10">
       <c r="A242" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B242" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E242" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F242" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G242" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="244" spans="1:10">
       <c r="A244" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E244" s="14" t="s">
         <v>41</v>
@@ -5410,21 +5365,21 @@
     </row>
     <row r="245" spans="1:10">
       <c r="A245" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B245" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E245" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G245" s="14" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="246" spans="1:10">
       <c r="A246" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B246" s="14" t="s">
         <v>8</v>
@@ -5438,7 +5393,7 @@
     </row>
     <row r="248" spans="1:10">
       <c r="A248" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D248" s="14" t="s">
         <v>20</v>
@@ -5458,7 +5413,7 @@
     </row>
     <row r="249" spans="1:10">
       <c r="A249" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B249" s="14" t="s">
         <v>33</v>
@@ -5473,7 +5428,7 @@
         <v>23</v>
       </c>
       <c r="I249" s="14" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="J249" s="14" t="s">
         <v>205</v>
@@ -5481,7 +5436,7 @@
     </row>
     <row r="250" spans="1:10">
       <c r="A250" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B250" s="14" t="s">
         <v>348</v>
@@ -5504,16 +5459,16 @@
     </row>
     <row r="252" spans="1:10">
       <c r="A252" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E252" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F252" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G252" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H252" s="14" t="s">
         <v>20</v>
@@ -5524,30 +5479,30 @@
     </row>
     <row r="253" spans="1:10">
       <c r="A253" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B253" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E253" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F253" s="14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G253" s="14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H253" s="14" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I253" s="14" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="254" spans="1:10">
       <c r="A254" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B254" s="14" t="s">
         <v>27</v>
@@ -5570,32 +5525,32 @@
     </row>
     <row r="256" spans="1:10">
       <c r="A256" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F256" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G256" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="257" spans="1:10">
       <c r="A257" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B257" s="14" t="s">
         <v>38</v>
       </c>
       <c r="F257" s="14" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G257" s="14" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="258" spans="1:10">
       <c r="A258" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B258" s="14" t="s">
         <v>8</v>
@@ -5609,7 +5564,7 @@
     </row>
     <row r="260" spans="1:10">
       <c r="A260" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D260" s="14" t="s">
         <v>20</v>
@@ -5632,7 +5587,7 @@
     </row>
     <row r="261" spans="1:10">
       <c r="A261" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B261" s="14" t="s">
         <v>38</v>
@@ -5658,44 +5613,44 @@
     </row>
     <row r="262" spans="1:10">
       <c r="A262" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B262" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D262" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E262" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F262" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H262" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I262" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J262" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="264" spans="1:10">
       <c r="A264" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F264" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="265" spans="1:10">
       <c r="A265" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B265" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F265" s="14" t="s">
         <v>288</v>
@@ -5703,7 +5658,7 @@
     </row>
     <row r="266" spans="1:10">
       <c r="A266" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B266" s="14" t="s">
         <v>253</v>
@@ -5714,24 +5669,21 @@
     </row>
     <row r="268" spans="1:10">
       <c r="A268" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D268" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G268" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="I268" s="14" t="s">
         <v>48</v>
       </c>
       <c r="J268" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="269" spans="1:10">
       <c r="A269" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B269" s="14" t="s">
         <v>38</v>
@@ -5739,9 +5691,6 @@
       <c r="D269" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G269" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="I269" s="14" t="s">
         <v>32</v>
       </c>
@@ -5751,7 +5700,7 @@
     </row>
     <row r="270" spans="1:10">
       <c r="A270" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B270" s="14" t="s">
         <v>8</v>
@@ -5759,11 +5708,8 @@
       <c r="D270" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G270" s="14" t="s">
-        <v>411</v>
-      </c>
       <c r="I270" s="14" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="J270" s="14" t="s">
         <v>31</v>
@@ -5771,7 +5717,7 @@
     </row>
     <row r="272" spans="1:10">
       <c r="A272" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D272" s="14" t="s">
         <v>33</v>
@@ -5788,13 +5734,13 @@
     </row>
     <row r="273" spans="1:10">
       <c r="A273" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B273" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D273" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G273" s="14" t="s">
         <v>39</v>
@@ -5808,7 +5754,7 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B274" s="14" t="s">
         <v>40</v>
@@ -5828,7 +5774,7 @@
     </row>
     <row r="276" spans="1:10">
       <c r="A276" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D276" s="14" t="s">
         <v>20</v>
@@ -5845,7 +5791,7 @@
     </row>
     <row r="277" spans="1:10">
       <c r="A277" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B277" s="14" t="s">
         <v>38</v>
@@ -5854,7 +5800,7 @@
         <v>39</v>
       </c>
       <c r="F277" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I277" s="14" t="s">
         <v>39</v>
@@ -5865,7 +5811,7 @@
     </row>
     <row r="278" spans="1:10">
       <c r="A278" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B278" s="14" t="s">
         <v>8</v>
@@ -5880,18 +5826,15 @@
         <v>40</v>
       </c>
       <c r="J278" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="280" spans="1:10">
       <c r="A280" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D280" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E280" s="14" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="F280" s="14" t="s">
         <v>51</v>
@@ -5900,7 +5843,7 @@
         <v>48</v>
       </c>
       <c r="I280" s="14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="J280" s="14" t="s">
         <v>48</v>
@@ -5908,59 +5851,53 @@
     </row>
     <row r="281" spans="1:10">
       <c r="A281" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B281" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D281" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E281" s="14" t="s">
-        <v>113</v>
+        <v>422</v>
       </c>
       <c r="F281" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G281" s="14" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="I281" s="14" t="s">
-        <v>54</v>
+        <v>422</v>
       </c>
       <c r="J281" s="14" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="282" spans="1:10">
       <c r="A282" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B282" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D282" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E282" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F282" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G282" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I282" s="14" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
       <c r="J282" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D284" s="14" t="s">
         <v>33</v>
@@ -5983,7 +5920,7 @@
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B285" s="14" t="s">
         <v>38</v>
@@ -5992,24 +5929,24 @@
         <v>252</v>
       </c>
       <c r="E285" s="14" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F285" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="H285" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="I285" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="J285" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B286" s="14" t="s">
         <v>8</v>
@@ -6035,7 +5972,7 @@
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D288" s="14" t="s">
         <v>33</v>
@@ -6050,35 +5987,35 @@
         <v>22</v>
       </c>
       <c r="J288" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="289" spans="1:10">
       <c r="A289" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B289" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D289" s="14" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F289" s="14" t="s">
         <v>287</v>
       </c>
       <c r="G289" s="14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I289" s="14" t="s">
         <v>287</v>
       </c>
       <c r="J289" s="14" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="290" spans="1:10">
       <c r="A290" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B290" s="14" t="s">
         <v>188</v>
@@ -6101,13 +6038,13 @@
     </row>
     <row r="292" spans="1:10">
       <c r="A292" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D292" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E292" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F292" s="14" t="s">
         <v>41</v>
@@ -6116,41 +6053,41 @@
         <v>41</v>
       </c>
       <c r="I292" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J292" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="293" spans="1:10">
       <c r="A293" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B293" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D293" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E293" s="14" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="F293" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="H293" s="14" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="I293" s="14" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="J293" s="14" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="294" spans="1:10">
       <c r="A294" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B294" s="14" t="s">
         <v>8</v>
@@ -6176,7 +6113,7 @@
     </row>
     <row r="296" spans="1:10">
       <c r="A296" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D296" s="14" t="s">
         <v>20</v>
@@ -6188,10 +6125,10 @@
         <v>20</v>
       </c>
       <c r="H296" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I296" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J296" s="14" t="s">
         <v>22</v>
@@ -6199,7 +6136,7 @@
     </row>
     <row r="297" spans="1:10">
       <c r="A297" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B297" s="14" t="s">
         <v>41</v>
@@ -6214,7 +6151,7 @@
         <v>39</v>
       </c>
       <c r="H297" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I297" s="14" t="s">
         <v>310</v>
@@ -6225,7 +6162,7 @@
     </row>
     <row r="298" spans="1:10">
       <c r="A298" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B298" s="14" t="s">
         <v>311</v>
@@ -6251,7 +6188,7 @@
     </row>
     <row r="300" spans="1:10">
       <c r="A300" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D300" s="14" t="s">
         <v>33</v>
@@ -6277,7 +6214,7 @@
         <v>41</v>
       </c>
       <c r="D301" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E301" s="14" t="s">
         <v>39</v>
@@ -6286,15 +6223,15 @@
         <v>39</v>
       </c>
       <c r="I301" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J301" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="302" spans="1:10">
       <c r="A302" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B302" s="14" t="s">
         <v>42</v>
@@ -6317,7 +6254,7 @@
     </row>
     <row r="304" spans="1:10">
       <c r="A304" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D304" s="14" t="s">
         <v>22</v>
@@ -6337,22 +6274,22 @@
     </row>
     <row r="305" spans="1:10">
       <c r="A305" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B305" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D305" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E305" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F305" s="14" t="s">
         <v>347</v>
       </c>
       <c r="I305" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J305" s="14" t="s">
         <v>336</v>
@@ -6360,36 +6297,36 @@
     </row>
     <row r="306" spans="1:10">
       <c r="A306" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="E306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="F306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="I306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="J306" s="14" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="308" spans="1:10">
       <c r="A308" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D308" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E308" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I308" s="14" t="s">
         <v>22</v>
@@ -6400,16 +6337,16 @@
     </row>
     <row r="309" spans="1:10">
       <c r="A309" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B309" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D309" s="14" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="E309" s="14" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="I309" s="14" t="s">
         <v>187</v>
@@ -6420,7 +6357,7 @@
     </row>
     <row r="310" spans="1:10">
       <c r="A310" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B310" s="14" t="s">
         <v>8</v>
@@ -6440,79 +6377,70 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D312" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E312" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F312" s="14" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="G312" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I312" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J312" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="313" spans="1:10">
       <c r="A313" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B313" s="14" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D313" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="G313" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="E313" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="G313" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="I313" s="14" t="s">
         <v>50</v>
       </c>
       <c r="J313" s="14" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="314" spans="1:10">
       <c r="A314" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D314" s="14" t="s">
-        <v>453</v>
-      </c>
-      <c r="E314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="F314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="G314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="I314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="J314" s="14" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="D316" s="14" t="s">
         <v>41</v>
@@ -6532,22 +6460,22 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B317" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D317" s="14" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="F317" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H317" s="14" t="s">
         <v>205</v>
       </c>
       <c r="I317" s="14" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="J317" s="14" t="s">
         <v>275</v>
@@ -6555,7 +6483,7 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B318" s="14" t="s">
         <v>259</v>
@@ -6564,46 +6492,46 @@
         <v>274</v>
       </c>
       <c r="F318" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H318" s="14" t="s">
         <v>259</v>
       </c>
       <c r="I318" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J318" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="320" spans="1:10">
       <c r="A320" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="G320" s="14" t="s">
         <v>22</v>
       </c>
       <c r="J320" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="321" spans="1:10">
       <c r="A321" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B321" s="14" t="s">
         <v>41</v>
       </c>
       <c r="G321" s="14" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="J321" s="14" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="322" spans="1:10">
       <c r="A322" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="B322" s="14" t="s">
         <v>240</v>
@@ -6617,7 +6545,7 @@
     </row>
     <row r="324" spans="1:10">
       <c r="A324" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="E324" s="14" t="s">
         <v>22</v>
@@ -6640,7 +6568,7 @@
     </row>
     <row r="325" spans="1:10">
       <c r="A325" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B325" s="14" t="s">
         <v>38</v>
@@ -6655,7 +6583,7 @@
         <v>39</v>
       </c>
       <c r="H325" s="14" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="I325" s="14" t="s">
         <v>304</v>
@@ -6666,7 +6594,7 @@
     </row>
     <row r="326" spans="1:10">
       <c r="A326" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B326" s="14" t="s">
         <v>8</v>
@@ -6675,7 +6603,7 @@
         <v>303</v>
       </c>
       <c r="F326" s="14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G326" s="14" t="s">
         <v>308</v>
@@ -6684,15 +6612,15 @@
         <v>303</v>
       </c>
       <c r="I326" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J326" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="J326" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="328" spans="1:10">
       <c r="A328" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D328" s="14" t="s">
         <v>33</v>
@@ -6712,30 +6640,30 @@
     </row>
     <row r="329" spans="1:10">
       <c r="A329" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B329" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D329" s="14" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="G329" s="14" t="s">
         <v>214</v>
       </c>
       <c r="H329" s="14" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="I329" s="14" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="J329" s="14" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="330" spans="1:10">
       <c r="A330" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="B330" s="14" t="s">
         <v>34</v>
@@ -6758,7 +6686,7 @@
     </row>
     <row r="332" spans="1:10">
       <c r="A332" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D332" s="14" t="s">
         <v>22</v>
@@ -6766,18 +6694,18 @@
     </row>
     <row r="333" spans="1:10">
       <c r="A333" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B333" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D333" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="334" spans="1:10">
       <c r="A334" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="B334" s="14" t="s">
         <v>8</v>
@@ -6788,13 +6716,13 @@
     </row>
     <row r="336" spans="1:10">
       <c r="A336" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D336" s="14" t="s">
         <v>20</v>
       </c>
       <c r="G336" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H336" s="14" t="s">
         <v>33</v>
@@ -6803,35 +6731,35 @@
         <v>20</v>
       </c>
       <c r="J336" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="337" spans="1:10">
       <c r="A337" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B337" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D337" s="14" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G337" s="14" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="H337" s="14" t="s">
         <v>296</v>
       </c>
       <c r="I337" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J337" s="14" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="338" spans="1:10">
       <c r="A338" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B338" s="14" t="s">
         <v>359</v>
@@ -6854,27 +6782,27 @@
     </row>
     <row r="340" spans="1:10">
       <c r="A340" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D340" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F340" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H340" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I340" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="341" spans="1:10">
       <c r="A341" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B341" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D341" s="14" t="s">
         <v>277</v>
@@ -6891,7 +6819,7 @@
     </row>
     <row r="342" spans="1:10">
       <c r="A342" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B342" s="14" t="s">
         <v>278</v>

</xml_diff>